<commit_message>
Add BD for HelloLL mems
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngocphat/git/discord-bot-minalinsky/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6238A7C-3E79-0A4D-8385-542248DA5EBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459145EC-6AD0-6745-83A6-F9E87974D740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="460" windowWidth="28040" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13920" yWindow="580" windowWidth="28040" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="216">
   <si>
     <t>date</t>
   </si>
@@ -653,6 +653,21 @@
   </si>
   <si>
     <t>µ's 6th</t>
+  </si>
+  <si>
+    <t>Hazuki Ren</t>
+  </si>
+  <si>
+    <t>Heanna Sumire</t>
+  </si>
+  <si>
+    <t>Arashi Chisato</t>
+  </si>
+  <si>
+    <t>Thảng Khửa Khừa</t>
+  </si>
+  <si>
+    <t>Shibuya Kanon</t>
   </si>
 </sst>
 </file>
@@ -1494,10 +1509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E98"/>
+  <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G89" sqref="G89"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3158,6 +3173,61 @@
         <v>207</v>
       </c>
     </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>40506</v>
+      </c>
+      <c r="B99" t="s">
+        <v>5</v>
+      </c>
+      <c r="C99" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>40449</v>
+      </c>
+      <c r="B100" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>40234</v>
+      </c>
+      <c r="B101" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102" s="1">
+        <v>40366</v>
+      </c>
+      <c r="B102" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>40299</v>
+      </c>
+      <c r="B103" t="s">
+        <v>5</v>
+      </c>
+      <c r="C103" t="s">
+        <v>215</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Sort Hello LL chars BD
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngocphat/git/discord-bot-minalinsky/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459145EC-6AD0-6745-83A6-F9E87974D740}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6333311-72DB-7E44-A245-1ED59A9DCB97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="580" windowWidth="28040" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="460" windowWidth="28040" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -1511,12 +1511,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C104" sqref="C104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
@@ -1796,81 +1797,75 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>40238</v>
+        <v>40234</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>40239</v>
+        <v>40238</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" t="s">
-        <v>209</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>208</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>40240</v>
+        <v>40239</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>209</v>
       </c>
       <c r="E19" t="s">
-        <v>47</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>40241</v>
+        <v>40240</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>40252</v>
+        <v>40241</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -1881,115 +1876,121 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>40254</v>
+        <v>40252</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>40262</v>
+        <v>40254</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23">
-        <v>2020</v>
-      </c>
-      <c r="E23">
-        <v>2020</v>
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>40271</v>
+        <v>40262</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>7</v>
+        <v>53</v>
+      </c>
+      <c r="D24">
+        <v>2020</v>
+      </c>
+      <c r="E24">
+        <v>2020</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>40273</v>
+        <v>40271</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25">
-        <v>2017</v>
-      </c>
-      <c r="E25">
-        <v>2017</v>
+        <v>54</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>40274</v>
+        <v>40273</v>
       </c>
       <c r="B26" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="D26">
+        <v>2017</v>
+      </c>
+      <c r="E26">
+        <v>2017</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>40283</v>
+        <v>40274</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="E27" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>40285</v>
+        <v>40283</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -2000,194 +2001,182 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>40287</v>
+        <v>40285</v>
       </c>
       <c r="B30" t="s">
         <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E30" t="s">
-        <v>7</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>40292</v>
+        <v>40287</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>66</v>
-      </c>
-      <c r="D31">
-        <v>2016</v>
-      </c>
-      <c r="E31">
-        <v>2016</v>
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>40293</v>
+        <v>40292</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" t="s">
-        <v>68</v>
-      </c>
-      <c r="E32" t="s">
-        <v>69</v>
+        <v>66</v>
+      </c>
+      <c r="D32">
+        <v>2016</v>
+      </c>
+      <c r="E32">
+        <v>2016</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>40300</v>
+        <v>40293</v>
       </c>
       <c r="B33" t="s">
         <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D33" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E33" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>40300</v>
+        <v>40299</v>
       </c>
       <c r="B34" t="s">
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" t="s">
-        <v>75</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>40302</v>
+        <v>40300</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>40309</v>
+        <v>40300</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E36" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>40317</v>
+        <v>40302</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E37" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>40328</v>
+        <v>40309</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="E38" t="s">
-        <v>7</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>40338</v>
+        <v>40317</v>
       </c>
       <c r="B39" t="s">
         <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>83</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>40342</v>
+        <v>40328</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
@@ -2198,13 +2187,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>40355</v>
+        <v>40338</v>
       </c>
       <c r="B41" t="s">
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
@@ -2215,248 +2204,242 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>40357</v>
+        <v>40342</v>
       </c>
       <c r="B42" t="s">
         <v>5</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D42" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>40359</v>
+        <v>40355</v>
       </c>
       <c r="B43" t="s">
-        <v>59</v>
+        <v>5</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
-      </c>
-      <c r="D43">
-        <v>2010</v>
+        <v>88</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>40361</v>
+        <v>40357</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D44" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E44" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>40371</v>
+        <v>40359</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
-      </c>
-      <c r="D45" t="s">
-        <v>97</v>
-      </c>
-      <c r="E45" t="s">
-        <v>98</v>
+        <v>92</v>
+      </c>
+      <c r="D45">
+        <v>2010</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>40372</v>
+        <v>40361</v>
       </c>
       <c r="B46" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="E46" t="s">
-        <v>7</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>40375</v>
+        <v>40366</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>100</v>
-      </c>
-      <c r="D47" t="s">
-        <v>101</v>
-      </c>
-      <c r="E47" t="s">
-        <v>102</v>
+        <v>214</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>40381</v>
+        <v>40371</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
       </c>
       <c r="C48" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>97</v>
       </c>
       <c r="E48" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>40381</v>
+        <v>40372</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C49" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D49" t="s">
-        <v>105</v>
+        <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>40382</v>
+        <v>40375</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D50" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="E50" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>40382</v>
+        <v>40381</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
       </c>
       <c r="C51" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D51" t="s">
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>40388</v>
+        <v>40381</v>
       </c>
       <c r="B52" t="s">
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E52" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>40391</v>
+        <v>40382</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
       </c>
       <c r="C53" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
       <c r="E53" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>40393</v>
+        <v>40382</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
       </c>
       <c r="C54" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D54" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E54" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>40396</v>
+        <v>40388</v>
       </c>
       <c r="B55" t="s">
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D55" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E55" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>40398</v>
+        <v>40391</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
@@ -2467,330 +2450,330 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>40398</v>
+        <v>40393</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D57" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E57" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>40406</v>
+        <v>40396</v>
       </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D58" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E58" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>40414</v>
+        <v>40398</v>
       </c>
       <c r="B59" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C59" t="s">
-        <v>129</v>
-      </c>
-      <c r="D59">
-        <v>2011</v>
-      </c>
-      <c r="E59">
-        <v>2011</v>
+        <v>122</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>40415</v>
+        <v>40398</v>
       </c>
       <c r="B60" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C60" t="s">
-        <v>130</v>
-      </c>
-      <c r="D60">
-        <v>2010</v>
-      </c>
-      <c r="E60">
-        <v>2010</v>
+        <v>123</v>
+      </c>
+      <c r="D60" t="s">
+        <v>124</v>
+      </c>
+      <c r="E60" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>40417</v>
+        <v>40406</v>
       </c>
       <c r="B61" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C61" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D61" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E61" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>40422</v>
+        <v>40414</v>
       </c>
       <c r="B62" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C62" t="s">
-        <v>134</v>
-      </c>
-      <c r="D62" t="s">
-        <v>135</v>
-      </c>
-      <c r="E62" t="s">
-        <v>136</v>
+        <v>129</v>
+      </c>
+      <c r="D62">
+        <v>2011</v>
+      </c>
+      <c r="E62">
+        <v>2011</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>40426</v>
+        <v>40415</v>
       </c>
       <c r="B63" t="s">
         <v>34</v>
       </c>
       <c r="C63" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D63">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="E63">
-        <v>2012</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>40428</v>
+        <v>40417</v>
       </c>
       <c r="B64" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D64" t="s">
-        <v>85</v>
+        <v>132</v>
       </c>
       <c r="E64" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>40431</v>
+        <v>40422</v>
       </c>
       <c r="B65" t="s">
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D65" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E65" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>40433</v>
+        <v>40426</v>
       </c>
       <c r="B66" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C66" t="s">
-        <v>143</v>
-      </c>
-      <c r="D66" t="s">
-        <v>7</v>
-      </c>
-      <c r="E66" t="s">
-        <v>7</v>
+        <v>137</v>
+      </c>
+      <c r="D66">
+        <v>2012</v>
+      </c>
+      <c r="E66">
+        <v>2012</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>40440</v>
+        <v>40428</v>
       </c>
       <c r="B67" t="s">
         <v>5</v>
       </c>
       <c r="C67" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="E67" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>40441</v>
+        <v>40431</v>
       </c>
       <c r="B68" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D68" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E68" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>40442</v>
+        <v>40433</v>
       </c>
       <c r="B69" t="s">
         <v>5</v>
       </c>
       <c r="C69" t="s">
-        <v>148</v>
+        <v>143</v>
+      </c>
+      <c r="D69" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>40445</v>
+        <v>40440</v>
       </c>
       <c r="B70" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C70" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D70" t="s">
-        <v>150</v>
+        <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>150</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>40446</v>
+        <v>40441</v>
       </c>
       <c r="B71" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C71" t="s">
-        <v>151</v>
-      </c>
-      <c r="D71">
-        <v>2019</v>
-      </c>
-      <c r="E71">
-        <v>2019</v>
+        <v>145</v>
+      </c>
+      <c r="D71" t="s">
+        <v>146</v>
+      </c>
+      <c r="E71" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>40446</v>
+        <v>40442</v>
       </c>
       <c r="B72" t="s">
         <v>5</v>
       </c>
       <c r="C72" t="s">
-        <v>152</v>
-      </c>
-      <c r="D72" t="s">
-        <v>153</v>
-      </c>
-      <c r="E72" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>40447</v>
+        <v>40445</v>
       </c>
       <c r="B73" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D73" t="s">
-        <v>7</v>
+        <v>150</v>
       </c>
       <c r="E73" t="s">
-        <v>7</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>40457</v>
+        <v>40446</v>
       </c>
       <c r="B74" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C74" t="s">
-        <v>156</v>
-      </c>
-      <c r="D74" t="s">
-        <v>157</v>
-      </c>
-      <c r="E74" t="s">
-        <v>158</v>
+        <v>151</v>
+      </c>
+      <c r="D74">
+        <v>2019</v>
+      </c>
+      <c r="E74">
+        <v>2019</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>40458</v>
+        <v>40446</v>
       </c>
       <c r="B75" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C75" t="s">
-        <v>159</v>
-      </c>
-      <c r="D75">
-        <v>2015</v>
-      </c>
-      <c r="E75">
-        <v>2015</v>
+        <v>152</v>
+      </c>
+      <c r="D75" t="s">
+        <v>153</v>
+      </c>
+      <c r="E75" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>40458</v>
+        <v>40447</v>
       </c>
       <c r="B76" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C76" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D76" t="s">
         <v>7</v>
@@ -2801,98 +2784,92 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>40467</v>
+        <v>40449</v>
       </c>
       <c r="B77" t="s">
         <v>5</v>
       </c>
       <c r="C77" t="s">
-        <v>161</v>
-      </c>
-      <c r="D77" t="s">
-        <v>162</v>
-      </c>
-      <c r="E77" t="s">
-        <v>163</v>
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>40472</v>
+        <v>40457</v>
       </c>
       <c r="B78" t="s">
         <v>5</v>
       </c>
       <c r="C78" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D78" t="s">
-        <v>7</v>
+        <v>157</v>
       </c>
       <c r="E78" t="s">
-        <v>7</v>
+        <v>158</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>40472</v>
+        <v>40458</v>
       </c>
       <c r="B79" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C79" t="s">
-        <v>165</v>
-      </c>
-      <c r="D79" t="s">
-        <v>166</v>
-      </c>
-      <c r="E79" t="s">
-        <v>167</v>
+        <v>159</v>
+      </c>
+      <c r="D79">
+        <v>2015</v>
+      </c>
+      <c r="E79">
+        <v>2015</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>40474</v>
+        <v>40458</v>
       </c>
       <c r="B80" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C80" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D80" t="s">
-        <v>169</v>
+        <v>7</v>
       </c>
       <c r="E80" t="s">
-        <v>170</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>40477</v>
+        <v>40467</v>
       </c>
       <c r="B81" t="s">
         <v>5</v>
       </c>
       <c r="C81" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D81" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="E81" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>40479</v>
+        <v>40472</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="D82" t="s">
         <v>7</v>
@@ -2903,332 +2880,359 @@
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>40481</v>
+        <v>40472</v>
       </c>
       <c r="B83" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>175</v>
-      </c>
-      <c r="D83">
-        <v>2019</v>
-      </c>
-      <c r="E83">
-        <v>2019</v>
+        <v>165</v>
+      </c>
+      <c r="D83" t="s">
+        <v>166</v>
+      </c>
+      <c r="E83" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>40483</v>
+        <v>40474</v>
       </c>
       <c r="B84" t="s">
         <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D84" t="s">
-        <v>7</v>
+        <v>169</v>
       </c>
       <c r="E84" t="s">
-        <v>7</v>
+        <v>170</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>40484</v>
+        <v>40477</v>
       </c>
       <c r="B85" t="s">
         <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D85" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E85" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>40493</v>
+        <v>40479</v>
       </c>
       <c r="B86" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C86" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D86" t="s">
-        <v>181</v>
+        <v>7</v>
       </c>
       <c r="E86" t="s">
-        <v>182</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>40495</v>
+        <v>40481</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C87" t="s">
-        <v>183</v>
-      </c>
-      <c r="D87" t="s">
-        <v>7</v>
-      </c>
-      <c r="E87" t="s">
-        <v>7</v>
+        <v>175</v>
+      </c>
+      <c r="D87">
+        <v>2019</v>
+      </c>
+      <c r="E87">
+        <v>2019</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>40500</v>
+        <v>40483</v>
       </c>
       <c r="B88" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D88" t="s">
-        <v>185</v>
+        <v>7</v>
       </c>
       <c r="E88" t="s">
-        <v>186</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>40509</v>
+        <v>40484</v>
       </c>
       <c r="B89" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="D89" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="E89" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>40509</v>
+        <v>40493</v>
       </c>
       <c r="B90" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="D90" t="s">
-        <v>210</v>
+        <v>181</v>
       </c>
       <c r="E90" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>40514</v>
+        <v>40495</v>
       </c>
       <c r="B91" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="D91" t="s">
-        <v>192</v>
+        <v>7</v>
       </c>
       <c r="E91" t="s">
-        <v>193</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>40522</v>
+        <v>40500</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C92" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="D92" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="E92" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>40527</v>
+        <v>40506</v>
       </c>
       <c r="B93" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>197</v>
-      </c>
-      <c r="D93" t="s">
-        <v>7</v>
-      </c>
-      <c r="E93" t="s">
-        <v>7</v>
+        <v>211</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>40528</v>
+        <v>40509</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C94" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="D94" t="s">
-        <v>7</v>
+        <v>188</v>
       </c>
       <c r="E94" t="s">
-        <v>7</v>
+        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>40534</v>
+        <v>40509</v>
       </c>
       <c r="B95" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C95" t="s">
-        <v>136</v>
-      </c>
-      <c r="D95">
-        <v>2010</v>
-      </c>
-      <c r="E95">
-        <v>2010</v>
+        <v>190</v>
+      </c>
+      <c r="D95" t="s">
+        <v>210</v>
+      </c>
+      <c r="E95" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>40535</v>
+        <v>40514</v>
       </c>
       <c r="B96" t="s">
         <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="D96" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E96" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>40538</v>
+        <v>40522</v>
       </c>
       <c r="B97" t="s">
         <v>5</v>
       </c>
       <c r="C97" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D97" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E97" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>40542</v>
+        <v>40527</v>
       </c>
       <c r="B98" t="s">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="C98" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D98" t="s">
-        <v>206</v>
+        <v>7</v>
       </c>
       <c r="E98" t="s">
-        <v>207</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>40506</v>
+        <v>40528</v>
       </c>
       <c r="B99" t="s">
         <v>5</v>
       </c>
       <c r="C99" t="s">
-        <v>211</v>
+        <v>198</v>
+      </c>
+      <c r="D99" t="s">
+        <v>7</v>
+      </c>
+      <c r="E99" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>40449</v>
+        <v>40534</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C100" t="s">
-        <v>212</v>
+        <v>136</v>
+      </c>
+      <c r="D100">
+        <v>2010</v>
+      </c>
+      <c r="E100">
+        <v>2010</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>40234</v>
+        <v>40535</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C101" t="s">
-        <v>213</v>
+        <v>199</v>
+      </c>
+      <c r="D101" t="s">
+        <v>200</v>
+      </c>
+      <c r="E101" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>40366</v>
+        <v>40538</v>
       </c>
       <c r="B102" t="s">
         <v>5</v>
       </c>
       <c r="C102" t="s">
-        <v>214</v>
+        <v>202</v>
+      </c>
+      <c r="D102" t="s">
+        <v>203</v>
+      </c>
+      <c r="E102" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>40299</v>
+        <v>40542</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>215</v>
+        <v>205</v>
+      </c>
+      <c r="D103" t="s">
+        <v>206</v>
+      </c>
+      <c r="E103" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E103">
+    <sortCondition ref="A84"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix Koizumi Moeka birthday
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ngocphat/git/discord-bot-minalinsky/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638BE236-37BF-B346-960C-5DB957422107}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965E9F19-4117-0740-B85C-41FB8DF6105C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="1020" windowWidth="28040" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="460" windowWidth="28040" windowHeight="16680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
@@ -1523,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E78" sqref="E78"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>43523</v>
+        <v>40236</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>

</xml_diff>